<commit_message>
defining todos and two more functions
</commit_message>
<xml_diff>
--- a/translation_table.xlsx
+++ b/translation_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Documents/GitHub/irrs_tool_py/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exactech-my.sharepoint.com/personal/aymee_rodriguez_exac_com/Documents/Projects/irrs_tool_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69CA4C7-9775-834B-BC7E-F157FD384188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{D69CA4C7-9775-834B-BC7E-F157FD384188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{685D3C65-956F-4C4F-8DBB-A83160201DB4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="224">
   <si>
     <t>the first | has to be replaced by {</t>
   </si>
@@ -689,13 +689,28 @@
   </si>
   <si>
     <t>symbol_incorrect_character</t>
+  </si>
+  <si>
+    <t>↔</t>
+  </si>
+  <si>
+    <t>ᴖ</t>
+  </si>
+  <si>
+    <t>⌓</t>
+  </si>
+  <si>
+    <t>↓</t>
+  </si>
+  <si>
+    <t>Ⓤ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +753,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Y14.5M-2009"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -759,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -776,6 +796,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,18 +1079,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>216</v>
       </c>
@@ -1080,7 +1101,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1120,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1152,7 +1173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1160,7 +1181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1168,7 +1189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1176,7 +1197,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1200,7 +1221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1208,7 +1229,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1224,7 +1245,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1232,7 +1253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1240,7 +1261,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1248,7 +1269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -1256,7 +1277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -1264,7 +1285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1272,7 +1293,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -1280,7 +1301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -1288,7 +1309,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>39</v>
       </c>
@@ -1296,7 +1317,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1320,7 +1341,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
@@ -1328,7 +1349,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1336,7 +1357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -1352,7 +1373,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -1368,7 +1389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -1376,7 +1397,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -1400,7 +1421,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1408,7 +1429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -1416,7 +1437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
@@ -1432,7 +1453,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -1440,7 +1461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -1448,7 +1469,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>59</v>
       </c>
@@ -1456,7 +1477,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1472,7 +1493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
@@ -1480,7 +1501,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -1488,7 +1509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -1496,7 +1517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>65</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -1512,7 +1533,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
@@ -1520,7 +1541,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>68</v>
       </c>
@@ -1528,7 +1549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -1536,7 +1557,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>70</v>
       </c>
@@ -1544,7 +1565,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>71</v>
       </c>
@@ -1552,7 +1573,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
@@ -1560,7 +1581,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
@@ -1574,7 +1595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -1582,7 +1603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>75</v>
       </c>
@@ -1590,7 +1611,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>76</v>
       </c>
@@ -1604,7 +1625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
@@ -1618,7 +1639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -1626,7 +1647,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>79</v>
       </c>
@@ -1634,7 +1655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>80</v>
       </c>
@@ -1642,7 +1663,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>81</v>
       </c>
@@ -1650,7 +1671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>82</v>
       </c>
@@ -1658,7 +1679,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>83</v>
       </c>
@@ -1666,7 +1687,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>84</v>
       </c>
@@ -1674,7 +1695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>85</v>
       </c>
@@ -1682,7 +1703,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>86</v>
       </c>
@@ -1690,7 +1711,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>87</v>
       </c>
@@ -1698,7 +1719,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>88</v>
       </c>
@@ -1706,7 +1727,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>89</v>
       </c>
@@ -1714,7 +1735,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -1722,7 +1743,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>91</v>
       </c>
@@ -1730,7 +1751,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>92</v>
       </c>
@@ -1738,7 +1759,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>93</v>
       </c>
@@ -1746,7 +1767,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>94</v>
       </c>
@@ -1754,7 +1775,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -1762,7 +1783,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -1770,7 +1791,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
@@ -1778,7 +1799,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>98</v>
       </c>
@@ -1786,7 +1807,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>99</v>
       </c>
@@ -1794,7 +1815,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
@@ -1802,7 +1823,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>101</v>
       </c>
@@ -1810,7 +1831,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>102</v>
       </c>
@@ -1818,7 +1839,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>103</v>
       </c>
@@ -1826,7 +1847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>104</v>
       </c>
@@ -1837,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>105</v>
       </c>
@@ -1848,7 +1869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>106</v>
       </c>
@@ -1859,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>107</v>
       </c>
@@ -1873,7 +1894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>108</v>
       </c>
@@ -1881,7 +1902,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>109</v>
       </c>
@@ -1889,7 +1910,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>110</v>
       </c>
@@ -1897,7 +1918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>111</v>
       </c>
@@ -1905,7 +1926,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>112</v>
       </c>
@@ -1913,7 +1934,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>113</v>
       </c>
@@ -1921,7 +1942,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>114</v>
       </c>
@@ -1929,7 +1950,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>115</v>
       </c>
@@ -1937,7 +1958,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>116</v>
       </c>
@@ -1945,7 +1966,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>117</v>
       </c>
@@ -1953,7 +1974,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>118</v>
       </c>
@@ -1961,7 +1982,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>119</v>
       </c>
@@ -1969,7 +1990,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>120</v>
       </c>
@@ -1977,7 +1998,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>121</v>
       </c>
@@ -1985,23 +2006,29 @@
         <v>121</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="C111" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="C112" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>124</v>
       </c>
@@ -2009,7 +2036,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>125</v>
       </c>
@@ -2017,7 +2044,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>126</v>
       </c>
@@ -2025,7 +2052,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>127</v>
       </c>
@@ -2033,7 +2060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>128</v>
       </c>
@@ -2041,7 +2068,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>129</v>
       </c>
@@ -2049,7 +2076,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>130</v>
       </c>
@@ -2057,7 +2084,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>131</v>
       </c>
@@ -2065,23 +2092,29 @@
         <v>131</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>134</v>
       </c>
@@ -2089,7 +2122,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>135</v>
       </c>
@@ -2097,7 +2130,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>136</v>
       </c>
@@ -2105,7 +2138,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>137</v>
       </c>
@@ -2113,7 +2146,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>138</v>
       </c>
@@ -2124,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>139</v>
       </c>
@@ -2132,7 +2165,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>140</v>
       </c>
@@ -2140,7 +2173,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>141</v>
       </c>
@@ -2148,7 +2181,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>142</v>
       </c>
@@ -2156,7 +2189,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>143</v>
       </c>
@@ -2164,7 +2197,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>144</v>
       </c>
@@ -2172,7 +2205,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>145</v>
       </c>
@@ -2180,7 +2213,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>146</v>
       </c>
@@ -2188,7 +2221,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>147</v>
       </c>
@@ -2196,15 +2229,18 @@
         <v>147</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -2212,7 +2248,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -2220,7 +2256,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>151</v>
       </c>
@@ -2231,7 +2267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>152</v>
       </c>
@@ -2239,7 +2275,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>153</v>
       </c>
@@ -2247,7 +2283,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>154</v>
       </c>
@@ -2255,7 +2291,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>155</v>
       </c>
@@ -2263,7 +2299,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>156</v>
       </c>
@@ -2271,7 +2307,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>157</v>
       </c>
@@ -2279,15 +2315,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="C147" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>159</v>
       </c>
@@ -2295,7 +2334,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>160</v>
       </c>
@@ -2303,7 +2342,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>161</v>
       </c>
@@ -2311,7 +2350,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>162</v>
       </c>
@@ -2319,15 +2358,18 @@
         <v>162</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="C152" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>164</v>
       </c>
@@ -2335,7 +2377,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>165</v>
       </c>
@@ -2343,7 +2385,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>166</v>
       </c>
@@ -2351,7 +2393,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>167</v>
       </c>
@@ -2359,7 +2401,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>168</v>
       </c>
@@ -2367,7 +2409,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>169</v>
       </c>
@@ -2375,7 +2417,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>170</v>
       </c>
@@ -2383,7 +2425,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>171</v>
       </c>
@@ -2391,7 +2433,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>172</v>
       </c>
@@ -2399,7 +2441,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>173</v>
       </c>
@@ -2407,7 +2449,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>174</v>
       </c>
@@ -2415,7 +2457,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>175</v>
       </c>
@@ -2423,7 +2465,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>176</v>
       </c>
@@ -2431,7 +2473,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>177</v>
       </c>
@@ -2439,7 +2481,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>178</v>
       </c>
@@ -2447,7 +2489,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>179</v>
       </c>
@@ -2455,7 +2497,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>180</v>
       </c>
@@ -2463,7 +2505,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>181</v>
       </c>
@@ -2471,7 +2513,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>182</v>
       </c>
@@ -2479,7 +2521,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>183</v>
       </c>
@@ -2487,7 +2529,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>184</v>
       </c>
@@ -2495,7 +2537,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>185</v>
       </c>
@@ -2503,7 +2545,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>186</v>
       </c>
@@ -2511,7 +2553,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>187</v>
       </c>
@@ -2519,7 +2561,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>188</v>
       </c>
@@ -2527,7 +2569,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>189</v>
       </c>
@@ -2535,7 +2577,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>190</v>
       </c>
@@ -2543,7 +2585,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>191</v>
       </c>
@@ -2551,7 +2593,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>192</v>
       </c>
@@ -2559,7 +2601,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>193</v>
       </c>
@@ -2567,7 +2609,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>194</v>
       </c>
@@ -2575,7 +2617,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>195</v>
       </c>
@@ -2583,7 +2625,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>196</v>
       </c>
@@ -2591,7 +2633,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>197</v>
       </c>
@@ -2599,7 +2641,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>198</v>
       </c>
@@ -2607,7 +2649,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>199</v>
       </c>
@@ -2615,7 +2657,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>200</v>
       </c>
@@ -2623,7 +2665,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>201</v>
       </c>
@@ -2631,7 +2673,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>202</v>
       </c>
@@ -2639,7 +2681,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>203</v>
       </c>
@@ -2647,7 +2689,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>204</v>
       </c>
@@ -2655,7 +2697,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -2663,7 +2705,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -2671,7 +2713,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>207</v>
       </c>
@@ -2679,7 +2721,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>208</v>
       </c>
@@ -2687,7 +2729,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>209</v>
       </c>
@@ -2695,7 +2737,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>210</v>
       </c>
@@ -2703,7 +2745,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>211</v>
       </c>
@@ -2711,7 +2753,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>212</v>
       </c>
@@ -2719,7 +2761,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>213</v>
       </c>
@@ -2727,7 +2769,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>214</v>
       </c>
@@ -2735,7 +2777,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>215</v>
       </c>
@@ -2745,6 +2787,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding engine for basic program functioning and correcting some cases
</commit_message>
<xml_diff>
--- a/translation_table.xlsx
+++ b/translation_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exactech-my.sharepoint.com/personal/aymee_rodriguez_exac_com/Documents/Projects/irrs_tool_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{D69CA4C7-9775-834B-BC7E-F157FD384188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{685D3C65-956F-4C4F-8DBB-A83160201DB4}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D69CA4C7-9775-834B-BC7E-F157FD384188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93053A25-3361-4C6C-913D-6D74EFC2C650}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="225">
   <si>
     <t>the first | has to be replaced by {</t>
   </si>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>Ⓤ</t>
+  </si>
+  <si>
+    <t>.\</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1480,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>65</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>68</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>70</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>71</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
@@ -1594,8 +1597,12 @@
       <c r="E62" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="F62" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>